<commit_message>
work with colon in translate
</commit_message>
<xml_diff>
--- a/original/Шторм_original.xlsx
+++ b/original/Шторм_original.xlsx
@@ -3379,12 +3379,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Please select the radius of the countermeasure zone (- meter)</t>
+          <t>Please select the radius of the countermeasure zone (unit: meter)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Пожалуйста, выберите радиус зоны противодействия (единица - метр)</t>
+          <t>Пожалуйста, выберите радиус зоны противодействия (единица измерения: метр)</t>
         </is>
       </c>
     </row>
@@ -3396,12 +3396,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Please select the radius of the defense area (- meter)</t>
+          <t>Please select the radius of the defense area (unit: meter)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Пожалуйста, выберите радиус зоны предупреждения (единица - метр)</t>
+          <t>Пожалуйста, выберите радиус зоны предупреждения (единица измерения: метр)</t>
         </is>
       </c>
     </row>
@@ -3697,12 +3697,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Frequency input - 70M - 6000M</t>
+          <t>Frequency input range: 70M - 6000M</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Диапазон ввода - 70M - 6000M</t>
+          <t>Диапазон ввода частоты: 70M - 6000M</t>
         </is>
       </c>
     </row>
@@ -4683,12 +4683,12 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>- You can search or manage the list of model references here.</t>
+          <t>Note: You can search or manage the list of model references here.</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>- Здесь вы можете искать или управлять списком ссылок на модели</t>
+          <t>Примечание: Здесь вы можете искать или управлять списком ссылок на модели</t>
         </is>
       </c>
     </row>

</xml_diff>